<commit_message>
scroll de las tablas funcional
</commit_message>
<xml_diff>
--- a/IA/asistencias/Tendencias_Tecnologicas.xlsx
+++ b/IA/asistencias/Tendencias_Tecnologicas.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,6 +415,9 @@
       <c r="D1" t="str">
         <v>2025-06-18</v>
       </c>
+      <c r="E1" t="str">
+        <v>2025-06-18</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -429,6 +432,9 @@
       <c r="D2" t="str">
         <v>✓</v>
       </c>
+      <c r="E2" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -443,6 +449,9 @@
       <c r="D3" t="str">
         <v>✓</v>
       </c>
+      <c r="E3" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -457,6 +466,9 @@
       <c r="D4" t="str">
         <v>✓</v>
       </c>
+      <c r="E4" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -471,6 +483,9 @@
       <c r="D5" t="str">
         <v>✓</v>
       </c>
+      <c r="E5" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -485,6 +500,9 @@
       <c r="D6" t="str">
         <v>✓</v>
       </c>
+      <c r="E6" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7">
@@ -499,6 +517,9 @@
       <c r="D7" t="str">
         <v>✓</v>
       </c>
+      <c r="E7" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8">
@@ -513,6 +534,9 @@
       <c r="D8" t="str">
         <v>✓</v>
       </c>
+      <c r="E8" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9">
@@ -527,6 +551,9 @@
       <c r="D9" t="str">
         <v>✓</v>
       </c>
+      <c r="E9" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10">
@@ -541,6 +568,9 @@
       <c r="D10" t="str">
         <v>✓</v>
       </c>
+      <c r="E10" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11">
@@ -555,6 +585,9 @@
       <c r="D11" t="str">
         <v>✓</v>
       </c>
+      <c r="E11" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -569,6 +602,9 @@
       <c r="D12" t="str">
         <v>✓</v>
       </c>
+      <c r="E12" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13">
@@ -583,6 +619,9 @@
       <c r="D13" t="str">
         <v>✓</v>
       </c>
+      <c r="E13" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14">
@@ -597,6 +636,9 @@
       <c r="D14" t="str">
         <v>✓</v>
       </c>
+      <c r="E14" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15">
@@ -611,6 +653,9 @@
       <c r="D15" t="str">
         <v>✓</v>
       </c>
+      <c r="E15" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16">
@@ -625,6 +670,9 @@
       <c r="D16" t="str">
         <v>✓</v>
       </c>
+      <c r="E16" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -639,10 +687,13 @@
       <c r="D17" t="str">
         <v>x</v>
       </c>
+      <c r="E17" t="str">
+        <v>x</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agregar correctamnete un nombre nuevo o lista
</commit_message>
<xml_diff>
--- a/IA/asistencias/Tendencias_Tecnologicas.xlsx
+++ b/IA/asistencias/Tendencias_Tecnologicas.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,6 +418,12 @@
       <c r="E1" t="str">
         <v>2025-06-18</v>
       </c>
+      <c r="F1" t="str">
+        <v>2025-06-18</v>
+      </c>
+      <c r="G1" t="str">
+        <v>2025-06-18</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -435,6 +441,12 @@
       <c r="E2" t="str">
         <v>✓</v>
       </c>
+      <c r="F2" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G2" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -452,6 +464,12 @@
       <c r="E3" t="str">
         <v>✓</v>
       </c>
+      <c r="F3" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G3" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -469,6 +487,12 @@
       <c r="E4" t="str">
         <v>✓</v>
       </c>
+      <c r="F4" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G4" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -486,6 +510,12 @@
       <c r="E5" t="str">
         <v>✓</v>
       </c>
+      <c r="F5" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G5" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -503,6 +533,12 @@
       <c r="E6" t="str">
         <v>✓</v>
       </c>
+      <c r="F6" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G6" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7">
@@ -520,6 +556,12 @@
       <c r="E7" t="str">
         <v>✓</v>
       </c>
+      <c r="F7" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G7" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8">
@@ -537,6 +579,12 @@
       <c r="E8" t="str">
         <v>✓</v>
       </c>
+      <c r="F8" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G8" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9">
@@ -554,6 +602,12 @@
       <c r="E9" t="str">
         <v>✓</v>
       </c>
+      <c r="F9" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G9" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10">
@@ -571,6 +625,12 @@
       <c r="E10" t="str">
         <v>✓</v>
       </c>
+      <c r="F10" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G10" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11">
@@ -588,6 +648,12 @@
       <c r="E11" t="str">
         <v>✓</v>
       </c>
+      <c r="F11" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G11" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -605,6 +671,12 @@
       <c r="E12" t="str">
         <v>✓</v>
       </c>
+      <c r="F12" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G12" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13">
@@ -622,6 +694,12 @@
       <c r="E13" t="str">
         <v>✓</v>
       </c>
+      <c r="F13" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G13" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14">
@@ -639,6 +717,12 @@
       <c r="E14" t="str">
         <v>✓</v>
       </c>
+      <c r="F14" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G14" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15">
@@ -656,6 +740,12 @@
       <c r="E15" t="str">
         <v>✓</v>
       </c>
+      <c r="F15" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G15" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16">
@@ -673,6 +763,12 @@
       <c r="E16" t="str">
         <v>✓</v>
       </c>
+      <c r="F16" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G16" t="str">
+        <v>✓</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -690,10 +786,108 @@
       <c r="E17" t="str">
         <v>x</v>
       </c>
+      <c r="F17" t="str">
+        <v>x</v>
+      </c>
+      <c r="G17" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>17</v>
+      </c>
+      <c r="B18" t="str">
+        <v xml:space="preserve">María Gómez </v>
+      </c>
+      <c r="C18" t="str">
+        <v>✓</v>
+      </c>
+      <c r="D18" t="str">
+        <v>✓</v>
+      </c>
+      <c r="E18" t="str">
+        <v>✓</v>
+      </c>
+      <c r="F18" t="str">
+        <v>x</v>
+      </c>
+      <c r="G18" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>18</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Santiago</v>
+      </c>
+      <c r="C19" t="str">
+        <v>✓</v>
+      </c>
+      <c r="D19" t="str">
+        <v>✓</v>
+      </c>
+      <c r="E19" t="str">
+        <v>✓</v>
+      </c>
+      <c r="F19" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G19" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>19</v>
+      </c>
+      <c r="B20" t="str">
+        <v xml:space="preserve">Robert </v>
+      </c>
+      <c r="C20" t="str">
+        <v>✓</v>
+      </c>
+      <c r="D20" t="str">
+        <v>✓</v>
+      </c>
+      <c r="E20" t="str">
+        <v>✓</v>
+      </c>
+      <c r="F20" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G20" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>20</v>
+      </c>
+      <c r="B21" t="str">
+        <v xml:space="preserve">Alfonso </v>
+      </c>
+      <c r="C21" t="str">
+        <v>x</v>
+      </c>
+      <c r="D21" t="str">
+        <v>x</v>
+      </c>
+      <c r="E21" t="str">
+        <v>x</v>
+      </c>
+      <c r="F21" t="str">
+        <v>✓</v>
+      </c>
+      <c r="G21" t="str">
+        <v>x</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G21"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>